<commit_message>
fix: unificacion de clases
</commit_message>
<xml_diff>
--- a/Tabla_simbolos.xlsx
+++ b/Tabla_simbolos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t xml:space="preserve">Tabla de literales/Pal. Reserv.</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">'!’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ Hola mundo }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; cadena</t>
   </si>
   <si>
     <t xml:space="preserve">'(‘</t>
@@ -532,14 +538,15 @@
   </sheetPr>
   <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
@@ -573,13 +580,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -596,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -619,7 +626,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>16</v>
@@ -636,13 +643,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>21</v>
+        <v>281</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>20</v>
@@ -653,13 +660,13 @@
         <v>21</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>22</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,13 +674,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>22</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,13 +688,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>23</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,13 +702,13 @@
         <v>27</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>23</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,13 +716,13 @@
         <v>29</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>21</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,18 +730,25 @@
         <v>31</v>
       </c>
       <c r="B13" s="4" t="n">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>284</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="4" t="n">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -742,36 +756,36 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4" t="n">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="n">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="n">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -779,10 +793,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="n">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -790,10 +804,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="n">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -801,10 +815,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4" t="n">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -812,10 +826,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="4" t="n">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -823,10 +837,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="4" t="n">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -834,10 +848,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="n">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -845,200 +859,200 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="n">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B25" s="4" t="n">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="4" t="n">
-        <v>122</v>
+        <v>257</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B27" s="4" t="n">
-        <v>123</v>
+        <v>258</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4" t="n">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B29" s="4" t="n">
-        <v>125</v>
+        <v>260</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="4" t="n">
-        <v>200</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31" s="4" t="n">
-        <v>201</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" s="4" t="n">
-        <v>202</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" s="4" t="n">
-        <v>203</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B34" s="4" t="n">
-        <v>204</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B35" s="4" t="n">
-        <v>205</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B36" s="4" t="n">
-        <v>206</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B37" s="4" t="n">
-        <v>207</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B38" s="4" t="n">
-        <v>208</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B39" s="4" t="n">
-        <v>209</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B40" s="4" t="n">
-        <v>210</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B41" s="4" t="n">
-        <v>211</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B42" s="4" t="n">
-        <v>212</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B43" s="4" t="n">
-        <v>213</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B44" s="4" t="n">
-        <v>214</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B45" s="4" t="n">
-        <v>215</v>
+        <v>276</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B47" s="10"/>
     </row>

</xml_diff>